<commit_message>
Input of urls through a text file on each line one by one accepted
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
-    <t>Analysis of FUNDS</t>
+    <t>Analysis of Funds</t>
   </si>
   <si>
     <t>Name of Fund</t>
@@ -55,10 +55,10 @@
     <t>8.53</t>
   </si>
   <si>
-    <t>10.62</t>
-  </si>
-  <si>
-    <t>12.14</t>
+    <t>9.31</t>
+  </si>
+  <si>
+    <t>11.69</t>
   </si>
   <si>
     <t>8.90</t>
@@ -76,13 +76,13 @@
     <t>0.30% (As on Oct 31, 2019)</t>
   </si>
   <si>
-    <t>10.26</t>
-  </si>
-  <si>
-    <t>11.53</t>
-  </si>
-  <si>
-    <t>7.64</t>
+    <t>10.29</t>
+  </si>
+  <si>
+    <t>11.35</t>
+  </si>
+  <si>
+    <t>7.63</t>
   </si>
   <si>
     <t>8.71</t>
@@ -109,15 +109,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -125,13 +137,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -438,8 +468,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
@@ -448,33 +478,36 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:8">
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -488,19 +521,19 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -514,23 +547,26 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="3" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D4:G4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>